<commit_message>
Combining measures and metrics derived from metadata.
</commit_message>
<xml_diff>
--- a/schema/Sisagua/issues_metadados_sisagua.xlsx
+++ b/schema/Sisagua/issues_metadados_sisagua.xlsx
@@ -7,11 +7,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="0_SCHEMA_METADATA" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="SCHEME_MEASURES" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="SCHEMA_METADATA" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="METADATA_MEASURES" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="METADATA_ISSUES" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="METADATA_MEASURES" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="METADATA_METRICS" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="METADATA_METRICS" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P47"/>
+  <dimension ref="A1:T47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,50 +469,70 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>DUPLICATED</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>NUM_ROWS</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>DATA_LENGTH</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>DATA_SCALE</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>AVG_COL_LEN</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>NUM_DISTINCT</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>NUM_NULLS</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>TABLE_ROWS</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>ROW_COUNT</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>NULLABLE</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>DEFAULT_ON_NULL</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>IS_PK</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>IS_FK</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>IS_UNIQUE</t>
         </is>
@@ -542,42 +561,56 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>CAMPO CHAVE DA TABELA</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>PK_GRAFICA (PRIMARY KEY, ENABLED); SYS_C001522203 (CHECK, ENABLED)</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
+          <t>PK_GRAFICA (PRIMARY KEY: ENABLED)- SYS_C0093984 (C: ENABLED)</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2" t="n">
         <v>22</v>
       </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
         <v>3</v>
       </c>
-      <c r="J2" t="n">
+      <c r="L2" t="n">
         <v>2</v>
       </c>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" t="b">
-        <v>0</v>
-      </c>
-      <c r="M2" t="b">
-        <v>0</v>
-      </c>
-      <c r="N2" t="b">
-        <v>1</v>
-      </c>
-      <c r="O2" t="b">
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
         <v>0</v>
       </c>
       <c r="P2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R2" t="b">
+        <v>1</v>
+      </c>
+      <c r="S2" t="b">
+        <v>0</v>
+      </c>
+      <c r="T2" t="b">
         <v>0</v>
       </c>
     </row>
@@ -604,42 +637,56 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>cod cnpj da gráfica</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>SYS_C001522204 (CHECK, ENABLED)</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
+          <t>SYS_C0093985 (C: ENABLED)</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" t="n">
         <v>22</v>
       </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
         <v>9</v>
       </c>
-      <c r="J3" t="n">
+      <c r="L3" t="n">
         <v>2</v>
       </c>
-      <c r="K3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M3" t="b">
-        <v>0</v>
-      </c>
-      <c r="N3" t="b">
-        <v>0</v>
-      </c>
-      <c r="O3" t="b">
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
         <v>0</v>
       </c>
       <c r="P3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="b">
+        <v>0</v>
+      </c>
+      <c r="R3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S3" t="b">
+        <v>0</v>
+      </c>
+      <c r="T3" t="b">
         <v>0</v>
       </c>
     </row>
@@ -666,42 +713,56 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>nome da gráfica</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>SYS_C001522205 (CHECK, ENABLED)</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
+          <t>SYS_C0093986 (C: ENABLED)</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>2</v>
+      </c>
+      <c r="I4" t="n">
         <v>80</v>
       </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
         <v>34</v>
       </c>
-      <c r="J4" t="n">
+      <c r="L4" t="n">
         <v>2</v>
       </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="b">
-        <v>0</v>
-      </c>
-      <c r="M4" t="b">
-        <v>0</v>
-      </c>
-      <c r="N4" t="b">
-        <v>0</v>
-      </c>
-      <c r="O4" t="b">
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
         <v>0</v>
       </c>
       <c r="P4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R4" t="b">
+        <v>0</v>
+      </c>
+      <c r="S4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T4" t="b">
         <v>0</v>
       </c>
     </row>
@@ -728,42 +789,56 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Data de início de atuação da gráfica para emissão de selos</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" t="n">
         <v>7</v>
       </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
         <v>8</v>
       </c>
-      <c r="J5" t="n">
+      <c r="L5" t="n">
         <v>2</v>
       </c>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" t="b">
-        <v>0</v>
-      </c>
-      <c r="M5" t="b">
-        <v>0</v>
-      </c>
-      <c r="N5" t="b">
-        <v>0</v>
-      </c>
-      <c r="O5" t="b">
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
         <v>0</v>
       </c>
       <c r="P5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R5" t="b">
+        <v>0</v>
+      </c>
+      <c r="S5" t="b">
+        <v>0</v>
+      </c>
+      <c r="T5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -790,42 +865,56 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Data de fim de atuação da gráfica para emissão de selos</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G6" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" t="n">
         <v>7</v>
       </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>1</v>
-      </c>
       <c r="J6" t="n">
         <v>0</v>
       </c>
       <c r="K6" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
         <v>2</v>
       </c>
-      <c r="L6" t="b">
-        <v>0</v>
-      </c>
-      <c r="M6" t="b">
-        <v>0</v>
-      </c>
-      <c r="N6" t="b">
-        <v>0</v>
-      </c>
-      <c r="O6" t="b">
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="n">
         <v>0</v>
       </c>
       <c r="P6" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q6" t="b">
+        <v>0</v>
+      </c>
+      <c r="R6" t="b">
+        <v>0</v>
+      </c>
+      <c r="S6" t="b">
+        <v>0</v>
+      </c>
+      <c r="T6" t="b">
         <v>0</v>
       </c>
     </row>
@@ -852,42 +941,56 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>status que indica se a gráfica está atualmente habilitada a emitir selos</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" t="n">
         <v>22</v>
       </c>
-      <c r="H7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
         <v>3</v>
       </c>
-      <c r="J7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" t="b">
-        <v>0</v>
-      </c>
-      <c r="M7" t="b">
-        <v>0</v>
-      </c>
-      <c r="N7" t="b">
-        <v>0</v>
-      </c>
-      <c r="O7" t="b">
+      <c r="L7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
         <v>0</v>
       </c>
       <c r="P7" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q7" t="b">
+        <v>0</v>
+      </c>
+      <c r="R7" t="b">
+        <v>0</v>
+      </c>
+      <c r="S7" t="b">
+        <v>0</v>
+      </c>
+      <c r="T7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -914,42 +1017,56 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>nome de usuário do sistema que terá acesso aos serviços da sefaz</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G8" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>2</v>
+      </c>
+      <c r="I8" t="n">
         <v>40</v>
       </c>
-      <c r="H8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
         <v>21</v>
       </c>
-      <c r="J8" t="n">
+      <c r="L8" t="n">
         <v>2</v>
       </c>
-      <c r="K8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" t="b">
-        <v>0</v>
-      </c>
-      <c r="M8" t="b">
-        <v>0</v>
-      </c>
-      <c r="N8" t="b">
-        <v>0</v>
-      </c>
-      <c r="O8" t="b">
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
         <v>0</v>
       </c>
       <c r="P8" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q8" t="b">
+        <v>0</v>
+      </c>
+      <c r="R8" t="b">
+        <v>0</v>
+      </c>
+      <c r="S8" t="b">
+        <v>0</v>
+      </c>
+      <c r="T8" t="b">
         <v>0</v>
       </c>
     </row>
@@ -976,42 +1093,56 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>senha de usuário do sistema que terá acesso aos serviços da sefaz</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G9" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" t="n">
         <v>25</v>
       </c>
-      <c r="H9" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
         <v>18</v>
       </c>
-      <c r="J9" t="n">
+      <c r="L9" t="n">
         <v>2</v>
       </c>
-      <c r="K9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" t="b">
-        <v>0</v>
-      </c>
-      <c r="M9" t="b">
-        <v>0</v>
-      </c>
-      <c r="N9" t="b">
-        <v>0</v>
-      </c>
-      <c r="O9" t="b">
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="n">
         <v>0</v>
       </c>
       <c r="P9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="b">
+        <v>0</v>
+      </c>
+      <c r="R9" t="b">
+        <v>0</v>
+      </c>
+      <c r="S9" t="b">
+        <v>0</v>
+      </c>
+      <c r="T9" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1038,42 +1169,56 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>URL dos serviços disponibilizados pela gráfica para acesso pela SEFAZ-CE</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G10" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>2</v>
+      </c>
+      <c r="I10" t="n">
         <v>300</v>
       </c>
-      <c r="H10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
         <v>60</v>
       </c>
-      <c r="J10" t="n">
+      <c r="L10" t="n">
         <v>2</v>
       </c>
-      <c r="K10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" t="b">
-        <v>0</v>
-      </c>
-      <c r="M10" t="b">
-        <v>0</v>
-      </c>
-      <c r="N10" t="b">
-        <v>0</v>
-      </c>
-      <c r="O10" t="b">
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="n">
         <v>0</v>
       </c>
       <c r="P10" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q10" t="b">
+        <v>0</v>
+      </c>
+      <c r="R10" t="b">
+        <v>0</v>
+      </c>
+      <c r="S10" t="b">
+        <v>0</v>
+      </c>
+      <c r="T10" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1105,37 +1250,51 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>PK_PEDIDO (PRIMARY KEY, ENABLED); SYS_C001240599 (CHECK, ENABLED)</t>
-        </is>
-      </c>
-      <c r="G11" t="n">
+          <t>PK_PEDIDO (PRIMARY KEY: ENABLED)- SYS_C00111558 (C: ENABLED)</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>328</v>
+      </c>
+      <c r="I11" t="n">
         <v>22</v>
       </c>
-      <c r="H11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" t="n">
-        <v>5</v>
-      </c>
       <c r="J11" t="n">
-        <v>17484</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
-      </c>
-      <c r="L11" t="b">
-        <v>0</v>
-      </c>
-      <c r="M11" t="b">
-        <v>0</v>
-      </c>
-      <c r="N11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O11" t="b">
+        <v>4</v>
+      </c>
+      <c r="L11" t="n">
+        <v>328</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" t="n">
         <v>0</v>
       </c>
       <c r="P11" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="b">
+        <v>0</v>
+      </c>
+      <c r="R11" t="b">
+        <v>1</v>
+      </c>
+      <c r="S11" t="b">
+        <v>0</v>
+      </c>
+      <c r="T11" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1162,42 +1321,56 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>código do pedido enviado pela gráfica</t>
+          <t>c�digo do pedido enviado pela gr�fica</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>SYS_C001240600 (CHECK, ENABLED)</t>
-        </is>
-      </c>
-      <c r="G12" t="n">
+          <t>SYS_C00111559 (C: ENABLED)</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>328</v>
+      </c>
+      <c r="I12" t="n">
         <v>22</v>
       </c>
-      <c r="H12" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
         <v>5</v>
       </c>
-      <c r="J12" t="n">
-        <v>17472</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0</v>
-      </c>
-      <c r="L12" t="b">
-        <v>0</v>
-      </c>
-      <c r="M12" t="b">
-        <v>0</v>
-      </c>
-      <c r="N12" t="b">
-        <v>0</v>
-      </c>
-      <c r="O12" t="b">
+      <c r="L12" t="n">
+        <v>324</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" t="n">
         <v>0</v>
       </c>
       <c r="P12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="b">
+        <v>0</v>
+      </c>
+      <c r="R12" t="b">
+        <v>0</v>
+      </c>
+      <c r="S12" t="b">
+        <v>0</v>
+      </c>
+      <c r="T12" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1229,37 +1402,51 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>SYS_C001240601 (CHECK, ENABLED)</t>
-        </is>
-      </c>
-      <c r="G13" t="n">
+          <t>SYS_C00111560 (C: ENABLED)</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>328</v>
+      </c>
+      <c r="I13" t="n">
         <v>22</v>
       </c>
-      <c r="H13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" t="n">
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
         <v>9</v>
       </c>
-      <c r="J13" t="n">
-        <v>249</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0</v>
-      </c>
-      <c r="L13" t="b">
-        <v>0</v>
-      </c>
-      <c r="M13" t="b">
-        <v>0</v>
-      </c>
-      <c r="N13" t="b">
-        <v>0</v>
-      </c>
-      <c r="O13" t="b">
+      <c r="L13" t="n">
+        <v>38</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" t="n">
         <v>0</v>
       </c>
       <c r="P13" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="b">
+        <v>0</v>
+      </c>
+      <c r="R13" t="b">
+        <v>0</v>
+      </c>
+      <c r="S13" t="b">
+        <v>0</v>
+      </c>
+      <c r="T13" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1286,7 +1473,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Tipo de água
+          <t xml:space="preserve">Tipo de �gua
 1-Mineral
 2-Adicionada de sais
 </t>
@@ -1294,37 +1481,51 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G14" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>328</v>
+      </c>
+      <c r="I14" t="n">
         <v>22</v>
       </c>
-      <c r="H14" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" t="n">
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
         <v>3</v>
       </c>
-      <c r="J14" t="n">
+      <c r="L14" t="n">
         <v>3</v>
       </c>
-      <c r="K14" t="n">
-        <v>0</v>
-      </c>
-      <c r="L14" t="b">
-        <v>0</v>
-      </c>
-      <c r="M14" t="b">
-        <v>0</v>
-      </c>
-      <c r="N14" t="b">
-        <v>0</v>
-      </c>
-      <c r="O14" t="b">
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" t="n">
         <v>0</v>
       </c>
       <c r="P14" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q14" t="b">
+        <v>0</v>
+      </c>
+      <c r="R14" t="b">
+        <v>0</v>
+      </c>
+      <c r="S14" t="b">
+        <v>0</v>
+      </c>
+      <c r="T14" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1351,44 +1552,58 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>INDICATIVO SE O SOLICITANTE É CREDENCIADO
-0-Não Credenciado
+          <t>INDICATIVO SE O SOLICITANTE � CREDENCIADO
+0-N�o Credenciado
 1-Credenciado</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G15" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>328</v>
+      </c>
+      <c r="I15" t="n">
         <v>22</v>
       </c>
-      <c r="H15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" t="n">
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
         <v>3</v>
       </c>
-      <c r="J15" t="n">
+      <c r="L15" t="n">
         <v>2</v>
       </c>
-      <c r="K15" t="n">
-        <v>0</v>
-      </c>
-      <c r="L15" t="b">
-        <v>0</v>
-      </c>
-      <c r="M15" t="b">
-        <v>0</v>
-      </c>
-      <c r="N15" t="b">
-        <v>0</v>
-      </c>
-      <c r="O15" t="b">
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
         <v>0</v>
       </c>
       <c r="P15" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q15" t="b">
+        <v>0</v>
+      </c>
+      <c r="R15" t="b">
+        <v>0</v>
+      </c>
+      <c r="S15" t="b">
+        <v>0</v>
+      </c>
+      <c r="T15" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1426,37 +1641,51 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G16" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>328</v>
+      </c>
+      <c r="I16" t="n">
         <v>22</v>
       </c>
-      <c r="H16" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" t="n">
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
         <v>3</v>
       </c>
-      <c r="J16" t="n">
+      <c r="L16" t="n">
         <v>5</v>
       </c>
-      <c r="K16" t="n">
-        <v>0</v>
-      </c>
-      <c r="L16" t="b">
-        <v>0</v>
-      </c>
-      <c r="M16" t="b">
-        <v>0</v>
-      </c>
-      <c r="N16" t="b">
-        <v>0</v>
-      </c>
-      <c r="O16" t="b">
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="n">
         <v>0</v>
       </c>
       <c r="P16" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q16" t="b">
+        <v>0</v>
+      </c>
+      <c r="R16" t="b">
+        <v>0</v>
+      </c>
+      <c r="S16" t="b">
+        <v>0</v>
+      </c>
+      <c r="T16" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1488,37 +1717,51 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G17" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>328</v>
+      </c>
+      <c r="I17" t="n">
         <v>22</v>
       </c>
-      <c r="H17" t="n">
+      <c r="J17" t="n">
         <v>2</v>
       </c>
-      <c r="I17" t="n">
+      <c r="K17" t="n">
         <v>4</v>
       </c>
-      <c r="J17" t="n">
-        <v>240</v>
-      </c>
-      <c r="K17" t="n">
-        <v>0</v>
-      </c>
-      <c r="L17" t="b">
-        <v>0</v>
-      </c>
-      <c r="M17" t="b">
-        <v>0</v>
-      </c>
-      <c r="N17" t="b">
-        <v>0</v>
-      </c>
-      <c r="O17" t="b">
+      <c r="L17" t="n">
+        <v>53</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" t="n">
         <v>0</v>
       </c>
       <c r="P17" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q17" t="b">
+        <v>0</v>
+      </c>
+      <c r="R17" t="b">
+        <v>0</v>
+      </c>
+      <c r="S17" t="b">
+        <v>0</v>
+      </c>
+      <c r="T17" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1550,37 +1793,51 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G18" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>328</v>
+      </c>
+      <c r="I18" t="n">
         <v>7</v>
       </c>
-      <c r="H18" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" t="n">
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" t="n">
         <v>8</v>
       </c>
-      <c r="J18" t="n">
-        <v>17484</v>
-      </c>
-      <c r="K18" t="n">
-        <v>0</v>
-      </c>
-      <c r="L18" t="b">
-        <v>0</v>
-      </c>
-      <c r="M18" t="b">
-        <v>0</v>
-      </c>
-      <c r="N18" t="b">
-        <v>0</v>
-      </c>
-      <c r="O18" t="b">
+      <c r="L18" t="n">
+        <v>327</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" t="n">
         <v>0</v>
       </c>
       <c r="P18" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q18" t="b">
+        <v>0</v>
+      </c>
+      <c r="R18" t="b">
+        <v>0</v>
+      </c>
+      <c r="S18" t="b">
+        <v>0</v>
+      </c>
+      <c r="T18" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1607,42 +1864,56 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Data do vencimento do débito gerado</t>
+          <t>Data do vencimento do d�bito gerado</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G19" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>328</v>
+      </c>
+      <c r="I19" t="n">
         <v>7</v>
       </c>
-      <c r="H19" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" t="n">
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" t="n">
         <v>8</v>
       </c>
-      <c r="J19" t="n">
-        <v>1925</v>
-      </c>
-      <c r="K19" t="n">
-        <v>0</v>
-      </c>
-      <c r="L19" t="b">
-        <v>0</v>
-      </c>
-      <c r="M19" t="b">
-        <v>0</v>
-      </c>
-      <c r="N19" t="b">
-        <v>0</v>
-      </c>
-      <c r="O19" t="b">
+      <c r="L19" t="n">
+        <v>69</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" t="n">
         <v>0</v>
       </c>
       <c r="P19" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q19" t="b">
+        <v>0</v>
+      </c>
+      <c r="R19" t="b">
+        <v>0</v>
+      </c>
+      <c r="S19" t="b">
+        <v>0</v>
+      </c>
+      <c r="T19" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1674,37 +1945,51 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G20" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>328</v>
+      </c>
+      <c r="I20" t="n">
         <v>22</v>
       </c>
-      <c r="H20" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" t="n">
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" t="n">
         <v>4</v>
       </c>
-      <c r="J20" t="n">
-        <v>120</v>
-      </c>
-      <c r="K20" t="n">
-        <v>0</v>
-      </c>
-      <c r="L20" t="b">
-        <v>0</v>
-      </c>
-      <c r="M20" t="b">
-        <v>0</v>
-      </c>
-      <c r="N20" t="b">
-        <v>0</v>
-      </c>
-      <c r="O20" t="b">
+      <c r="L20" t="n">
+        <v>33</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" t="n">
         <v>0</v>
       </c>
       <c r="P20" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R20" t="b">
+        <v>0</v>
+      </c>
+      <c r="S20" t="b">
+        <v>0</v>
+      </c>
+      <c r="T20" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1731,42 +2016,56 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>código do débito gerado no copaf</t>
+          <t>c�digo do d�bito gerado no copaf</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G21" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>328</v>
+      </c>
+      <c r="I21" t="n">
         <v>22</v>
       </c>
-      <c r="H21" t="n">
-        <v>0</v>
-      </c>
-      <c r="I21" t="n">
+      <c r="J21" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" t="n">
         <v>4</v>
       </c>
-      <c r="J21" t="n">
-        <v>9071</v>
-      </c>
-      <c r="K21" t="n">
-        <v>8413</v>
-      </c>
-      <c r="L21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N21" t="b">
-        <v>0</v>
-      </c>
-      <c r="O21" t="b">
+      <c r="L21" t="n">
+        <v>173</v>
+      </c>
+      <c r="M21" t="n">
+        <v>150</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0</v>
+      </c>
+      <c r="O21" t="n">
         <v>0</v>
       </c>
       <c r="P21" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q21" t="b">
+        <v>0</v>
+      </c>
+      <c r="R21" t="b">
+        <v>0</v>
+      </c>
+      <c r="S21" t="b">
+        <v>0</v>
+      </c>
+      <c r="T21" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1798,37 +2097,51 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G22" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>328</v>
+      </c>
+      <c r="I22" t="n">
         <v>44</v>
       </c>
-      <c r="H22" t="n">
-        <v>0</v>
-      </c>
-      <c r="I22" t="n">
-        <v>37</v>
-      </c>
       <c r="J22" t="n">
-        <v>14133</v>
+        <v>0</v>
       </c>
       <c r="K22" t="n">
-        <v>3330</v>
-      </c>
-      <c r="L22" t="b">
-        <v>0</v>
-      </c>
-      <c r="M22" t="b">
-        <v>0</v>
-      </c>
-      <c r="N22" t="b">
-        <v>0</v>
-      </c>
-      <c r="O22" t="b">
+        <v>6</v>
+      </c>
+      <c r="L22" t="n">
+        <v>30</v>
+      </c>
+      <c r="M22" t="n">
+        <v>298</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0</v>
+      </c>
+      <c r="O22" t="n">
         <v>0</v>
       </c>
       <c r="P22" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q22" t="b">
+        <v>0</v>
+      </c>
+      <c r="R22" t="b">
+        <v>0</v>
+      </c>
+      <c r="S22" t="b">
+        <v>0</v>
+      </c>
+      <c r="T22" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1856,43 +2169,57 @@
       <c r="E23" t="inlineStr">
         <is>
           <t>INDICATIVO SE O SOLICITANTE POSSUI REGIME ESPECIAL
-0-Não Possui Regime Especial
+0-N�o Possui Regime Especial
 1-Possui Regime Especial</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G23" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>328</v>
+      </c>
+      <c r="I23" t="n">
         <v>22</v>
       </c>
-      <c r="H23" t="n">
-        <v>0</v>
-      </c>
-      <c r="I23" t="n">
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" t="n">
         <v>3</v>
       </c>
-      <c r="J23" t="n">
+      <c r="L23" t="n">
         <v>2</v>
       </c>
-      <c r="K23" t="n">
-        <v>0</v>
-      </c>
-      <c r="L23" t="b">
-        <v>0</v>
-      </c>
-      <c r="M23" t="b">
-        <v>0</v>
-      </c>
-      <c r="N23" t="b">
-        <v>0</v>
-      </c>
-      <c r="O23" t="b">
+      <c r="M23" t="n">
+        <v>7</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" t="n">
         <v>0</v>
       </c>
       <c r="P23" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q23" t="b">
+        <v>0</v>
+      </c>
+      <c r="R23" t="b">
+        <v>0</v>
+      </c>
+      <c r="S23" t="b">
+        <v>0</v>
+      </c>
+      <c r="T23" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1919,42 +2246,56 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Valor unitário do Selo para o pedido</t>
+          <t>Valor unit�rio do Selo para o pedido</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G24" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>328</v>
+      </c>
+      <c r="I24" t="n">
         <v>22</v>
       </c>
-      <c r="H24" t="n">
+      <c r="J24" t="n">
         <v>2</v>
       </c>
-      <c r="I24" t="n">
+      <c r="K24" t="n">
         <v>3</v>
       </c>
-      <c r="J24" t="n">
-        <v>8</v>
-      </c>
-      <c r="K24" t="n">
-        <v>0</v>
-      </c>
-      <c r="L24" t="b">
-        <v>0</v>
-      </c>
-      <c r="M24" t="b">
-        <v>0</v>
-      </c>
-      <c r="N24" t="b">
-        <v>0</v>
-      </c>
-      <c r="O24" t="b">
+      <c r="L24" t="n">
+        <v>12</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" t="n">
         <v>0</v>
       </c>
       <c r="P24" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q24" t="b">
+        <v>0</v>
+      </c>
+      <c r="R24" t="b">
+        <v>0</v>
+      </c>
+      <c r="S24" t="b">
+        <v>0</v>
+      </c>
+      <c r="T24" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1981,42 +2322,56 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>chave estrangeira - sequencial da gráfica onde o pedido foi originado</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>FK_GRA_R_PED (FOREIGN KEY, ENABLED); SYS_C001522213 (CHECK, ENABLED)</t>
-        </is>
-      </c>
-      <c r="G25" t="n">
+          <t>FK_GRA_R_PED (FOREIGN KEY: ENABLED)</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>328</v>
+      </c>
+      <c r="I25" t="n">
         <v>22</v>
       </c>
-      <c r="H25" t="n">
-        <v>0</v>
-      </c>
-      <c r="I25" t="n">
+      <c r="J25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="n">
         <v>3</v>
       </c>
-      <c r="J25" t="n">
+      <c r="L25" t="n">
         <v>2</v>
       </c>
-      <c r="K25" t="n">
-        <v>0</v>
-      </c>
-      <c r="L25" t="b">
-        <v>0</v>
-      </c>
-      <c r="M25" t="b">
-        <v>0</v>
-      </c>
-      <c r="N25" t="b">
-        <v>0</v>
-      </c>
-      <c r="O25" t="b">
-        <v>1</v>
+      <c r="M25" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0</v>
       </c>
       <c r="P25" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q25" t="b">
+        <v>0</v>
+      </c>
+      <c r="R25" t="b">
+        <v>0</v>
+      </c>
+      <c r="S25" t="b">
+        <v>1</v>
+      </c>
+      <c r="T25" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2043,42 +2398,56 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Campo responsável por identificar uma solicitação de criação de débito  no sistema de conta corrente.</t>
+          <t>Campo respons�vel por identificar uma solicita��o de cria��o de d�bito  no sistema de conta corrente.</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G26" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>328</v>
+      </c>
+      <c r="I26" t="n">
         <v>36</v>
       </c>
-      <c r="H26" t="n">
-        <v>0</v>
-      </c>
-      <c r="I26" t="n">
-        <v>0</v>
-      </c>
       <c r="J26" t="n">
         <v>0</v>
       </c>
       <c r="K26" t="n">
-        <v>17484</v>
-      </c>
-      <c r="L26" t="b">
-        <v>0</v>
-      </c>
-      <c r="M26" t="b">
-        <v>0</v>
-      </c>
-      <c r="N26" t="b">
-        <v>0</v>
-      </c>
-      <c r="O26" t="b">
+        <v>14</v>
+      </c>
+      <c r="L26" t="n">
+        <v>111</v>
+      </c>
+      <c r="M26" t="n">
+        <v>217</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0</v>
+      </c>
+      <c r="O26" t="n">
         <v>0</v>
       </c>
       <c r="P26" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q26" t="b">
+        <v>0</v>
+      </c>
+      <c r="R26" t="b">
+        <v>0</v>
+      </c>
+      <c r="S26" t="b">
+        <v>0</v>
+      </c>
+      <c r="T26" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2105,42 +2474,56 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Campo chave primaria da tabela que irá utilizar a sequence SEQ_DEBITO.</t>
+          <t>Campo chave primaria da tabela que ir� utilizar a sequence SEQ_DEBITO.</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>FK_DEBITO_R_PEDIDO (FOREIGN KEY, ENABLED)</t>
-        </is>
-      </c>
-      <c r="G27" t="n">
+          <t>FK_DEBITO_R_PEDIDO (FOREIGN KEY: ENABLED)</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
+        <v>328</v>
+      </c>
+      <c r="I27" t="n">
         <v>22</v>
       </c>
-      <c r="H27" t="n">
-        <v>0</v>
-      </c>
-      <c r="I27" t="n">
-        <v>4</v>
-      </c>
       <c r="J27" t="n">
-        <v>8532</v>
+        <v>0</v>
       </c>
       <c r="K27" t="n">
-        <v>8952</v>
-      </c>
-      <c r="L27" t="b">
-        <v>0</v>
-      </c>
-      <c r="M27" t="b">
-        <v>0</v>
-      </c>
-      <c r="N27" t="b">
-        <v>0</v>
-      </c>
-      <c r="O27" t="b">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="L27" t="n">
+        <v>17</v>
+      </c>
+      <c r="M27" t="n">
+        <v>311</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0</v>
       </c>
       <c r="P27" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q27" t="b">
+        <v>0</v>
+      </c>
+      <c r="R27" t="b">
+        <v>0</v>
+      </c>
+      <c r="S27" t="b">
+        <v>1</v>
+      </c>
+      <c r="T27" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2172,37 +2555,51 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>FK_PED_GRA_R_PED_FLU (FOREIGN KEY, ENABLED)</t>
-        </is>
-      </c>
-      <c r="G28" t="n">
+          <t>FK_PED_GRA_R_PED_FLU (FOREIGN KEY: ENABLED)</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
+        <v>4459</v>
+      </c>
+      <c r="I28" t="n">
         <v>22</v>
       </c>
-      <c r="H28" t="n">
-        <v>0</v>
-      </c>
-      <c r="I28" t="n">
+      <c r="J28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" t="n">
         <v>4</v>
       </c>
-      <c r="J28" t="n">
-        <v>3159</v>
-      </c>
-      <c r="K28" t="n">
-        <v>0</v>
-      </c>
-      <c r="L28" t="b">
-        <v>0</v>
-      </c>
-      <c r="M28" t="b">
-        <v>0</v>
-      </c>
-      <c r="N28" t="b">
-        <v>0</v>
-      </c>
-      <c r="O28" t="b">
-        <v>1</v>
+      <c r="L28" t="n">
+        <v>662</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0</v>
+      </c>
+      <c r="O28" t="n">
+        <v>0</v>
       </c>
       <c r="P28" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q28" t="b">
+        <v>0</v>
+      </c>
+      <c r="R28" t="b">
+        <v>0</v>
+      </c>
+      <c r="S28" t="b">
+        <v>1</v>
+      </c>
+      <c r="T28" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2229,42 +2626,56 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>DATA A AÇÃO DO FLUXO</t>
+          <t>DATA A A��O DO FLUXO</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G29" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H29" t="n">
+        <v>4459</v>
+      </c>
+      <c r="I29" t="n">
         <v>7</v>
       </c>
-      <c r="H29" t="n">
-        <v>0</v>
-      </c>
-      <c r="I29" t="n">
+      <c r="J29" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" t="n">
         <v>8</v>
       </c>
-      <c r="J29" t="n">
-        <v>19440</v>
-      </c>
-      <c r="K29" t="n">
-        <v>0</v>
-      </c>
-      <c r="L29" t="b">
-        <v>0</v>
-      </c>
-      <c r="M29" t="b">
-        <v>0</v>
-      </c>
-      <c r="N29" t="b">
-        <v>0</v>
-      </c>
-      <c r="O29" t="b">
+      <c r="L29" t="n">
+        <v>3625</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0</v>
+      </c>
+      <c r="O29" t="n">
         <v>0</v>
       </c>
       <c r="P29" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q29" t="b">
+        <v>0</v>
+      </c>
+      <c r="R29" t="b">
+        <v>0</v>
+      </c>
+      <c r="S29" t="b">
+        <v>0</v>
+      </c>
+      <c r="T29" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2291,42 +2702,56 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>DESCRIÇÃO DA AÇÃO DO FLUXO</t>
+          <t>DESCRI��O DA A��O DO FLUXO</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G30" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>4459</v>
+      </c>
+      <c r="I30" t="n">
         <v>2000</v>
       </c>
-      <c r="H30" t="n">
-        <v>0</v>
-      </c>
-      <c r="I30" t="n">
-        <v>45</v>
-      </c>
       <c r="J30" t="n">
-        <v>2956</v>
+        <v>0</v>
       </c>
       <c r="K30" t="n">
-        <v>1</v>
-      </c>
-      <c r="L30" t="b">
-        <v>0</v>
-      </c>
-      <c r="M30" t="b">
-        <v>0</v>
-      </c>
-      <c r="N30" t="b">
-        <v>0</v>
-      </c>
-      <c r="O30" t="b">
+        <v>40</v>
+      </c>
+      <c r="L30" t="n">
+        <v>564</v>
+      </c>
+      <c r="M30" t="n">
+        <v>1</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" t="n">
         <v>0</v>
       </c>
       <c r="P30" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q30" t="b">
+        <v>0</v>
+      </c>
+      <c r="R30" t="b">
+        <v>0</v>
+      </c>
+      <c r="S30" t="b">
+        <v>0</v>
+      </c>
+      <c r="T30" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2358,37 +2783,51 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G31" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H31" t="n">
+        <v>4459</v>
+      </c>
+      <c r="I31" t="n">
         <v>7</v>
       </c>
-      <c r="H31" t="n">
-        <v>0</v>
-      </c>
-      <c r="I31" t="n">
+      <c r="J31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" t="n">
         <v>8</v>
       </c>
-      <c r="J31" t="n">
-        <v>394</v>
-      </c>
-      <c r="K31" t="n">
-        <v>0</v>
-      </c>
-      <c r="L31" t="b">
-        <v>0</v>
-      </c>
-      <c r="M31" t="b">
-        <v>0</v>
-      </c>
-      <c r="N31" t="b">
-        <v>0</v>
-      </c>
-      <c r="O31" t="b">
+      <c r="L31" t="n">
+        <v>2</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0</v>
+      </c>
+      <c r="O31" t="n">
         <v>0</v>
       </c>
       <c r="P31" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q31" t="b">
+        <v>0</v>
+      </c>
+      <c r="R31" t="b">
+        <v>0</v>
+      </c>
+      <c r="S31" t="b">
+        <v>0</v>
+      </c>
+      <c r="T31" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2420,37 +2859,51 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>PK_PEDIDO_GRAFICA (PRIMARY KEY, ENABLED); SYS_C001330918 (CHECK, ENABLED)</t>
-        </is>
-      </c>
-      <c r="G32" t="n">
+          <t>PK_PEDIDO_GRAFICA (PRIMARY KEY: ENABLED)- SYS_C00106664 (C: ENABLED)</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H32" t="n">
+        <v>662</v>
+      </c>
+      <c r="I32" t="n">
         <v>22</v>
       </c>
-      <c r="H32" t="n">
-        <v>0</v>
-      </c>
-      <c r="I32" t="n">
+      <c r="J32" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" t="n">
         <v>4</v>
       </c>
-      <c r="J32" t="n">
-        <v>3159</v>
-      </c>
-      <c r="K32" t="n">
-        <v>0</v>
-      </c>
-      <c r="L32" t="b">
-        <v>0</v>
-      </c>
-      <c r="M32" t="b">
-        <v>0</v>
-      </c>
-      <c r="N32" t="b">
-        <v>1</v>
-      </c>
-      <c r="O32" t="b">
+      <c r="L32" t="n">
+        <v>662</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0</v>
+      </c>
+      <c r="O32" t="n">
         <v>0</v>
       </c>
       <c r="P32" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q32" t="b">
+        <v>0</v>
+      </c>
+      <c r="R32" t="b">
+        <v>1</v>
+      </c>
+      <c r="S32" t="b">
+        <v>0</v>
+      </c>
+      <c r="T32" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2477,42 +2930,56 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>CÓDIGO DO PEDIDO</t>
+          <t>C�DIGO DO PEDIDO</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G33" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>662</v>
+      </c>
+      <c r="I33" t="n">
         <v>22</v>
       </c>
-      <c r="H33" t="n">
-        <v>0</v>
-      </c>
-      <c r="I33" t="n">
+      <c r="J33" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" t="n">
         <v>4</v>
       </c>
-      <c r="J33" t="n">
-        <v>3159</v>
-      </c>
-      <c r="K33" t="n">
-        <v>0</v>
-      </c>
-      <c r="L33" t="b">
-        <v>0</v>
-      </c>
-      <c r="M33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N33" t="b">
-        <v>0</v>
-      </c>
-      <c r="O33" t="b">
+      <c r="L33" t="n">
+        <v>662</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0</v>
+      </c>
+      <c r="O33" t="n">
         <v>0</v>
       </c>
       <c r="P33" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q33" t="b">
+        <v>0</v>
+      </c>
+      <c r="R33" t="b">
+        <v>0</v>
+      </c>
+      <c r="S33" t="b">
+        <v>0</v>
+      </c>
+      <c r="T33" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2544,37 +3011,51 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G34" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>662</v>
+      </c>
+      <c r="I34" t="n">
         <v>7</v>
       </c>
-      <c r="H34" t="n">
-        <v>0</v>
-      </c>
-      <c r="I34" t="n">
+      <c r="J34" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" t="n">
         <v>8</v>
       </c>
-      <c r="J34" t="n">
-        <v>3081</v>
-      </c>
-      <c r="K34" t="n">
-        <v>0</v>
-      </c>
-      <c r="L34" t="b">
-        <v>0</v>
-      </c>
-      <c r="M34" t="b">
-        <v>0</v>
-      </c>
-      <c r="N34" t="b">
-        <v>0</v>
-      </c>
-      <c r="O34" t="b">
+      <c r="L34" t="n">
+        <v>660</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0</v>
+      </c>
+      <c r="O34" t="n">
         <v>0</v>
       </c>
       <c r="P34" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q34" t="b">
+        <v>0</v>
+      </c>
+      <c r="R34" t="b">
+        <v>0</v>
+      </c>
+      <c r="S34" t="b">
+        <v>0</v>
+      </c>
+      <c r="T34" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2606,37 +3087,51 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G35" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>662</v>
+      </c>
+      <c r="I35" t="n">
         <v>22</v>
       </c>
-      <c r="H35" t="n">
-        <v>0</v>
-      </c>
-      <c r="I35" t="n">
+      <c r="J35" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" t="n">
         <v>9</v>
       </c>
-      <c r="J35" t="n">
-        <v>183</v>
-      </c>
-      <c r="K35" t="n">
-        <v>1</v>
-      </c>
-      <c r="L35" t="b">
-        <v>0</v>
-      </c>
-      <c r="M35" t="b">
-        <v>0</v>
-      </c>
-      <c r="N35" t="b">
-        <v>0</v>
-      </c>
-      <c r="O35" t="b">
+      <c r="L35" t="n">
+        <v>133</v>
+      </c>
+      <c r="M35" t="n">
+        <v>1</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0</v>
+      </c>
+      <c r="O35" t="n">
         <v>0</v>
       </c>
       <c r="P35" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q35" t="b">
+        <v>0</v>
+      </c>
+      <c r="R35" t="b">
+        <v>0</v>
+      </c>
+      <c r="S35" t="b">
+        <v>0</v>
+      </c>
+      <c r="T35" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2663,42 +3158,56 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>RAQZÃO SOCIAL DO SOLICITANTE</t>
+          <t>RAQZ�O SOCIAL DO SOLICITANTE</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G36" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>662</v>
+      </c>
+      <c r="I36" t="n">
         <v>200</v>
       </c>
-      <c r="H36" t="n">
-        <v>0</v>
-      </c>
-      <c r="I36" t="n">
-        <v>40</v>
-      </c>
       <c r="J36" t="n">
-        <v>182</v>
+        <v>0</v>
       </c>
       <c r="K36" t="n">
-        <v>1</v>
-      </c>
-      <c r="L36" t="b">
-        <v>0</v>
-      </c>
-      <c r="M36" t="b">
-        <v>0</v>
-      </c>
-      <c r="N36" t="b">
-        <v>0</v>
-      </c>
-      <c r="O36" t="b">
+        <v>39</v>
+      </c>
+      <c r="L36" t="n">
+        <v>132</v>
+      </c>
+      <c r="M36" t="n">
+        <v>1</v>
+      </c>
+      <c r="N36" t="n">
+        <v>0</v>
+      </c>
+      <c r="O36" t="n">
         <v>0</v>
       </c>
       <c r="P36" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q36" t="b">
+        <v>0</v>
+      </c>
+      <c r="R36" t="b">
+        <v>0</v>
+      </c>
+      <c r="S36" t="b">
+        <v>0</v>
+      </c>
+      <c r="T36" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2730,37 +3239,51 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G37" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
+        <v>662</v>
+      </c>
+      <c r="I37" t="n">
         <v>22</v>
       </c>
-      <c r="H37" t="n">
-        <v>0</v>
-      </c>
-      <c r="I37" t="n">
+      <c r="J37" t="n">
+        <v>0</v>
+      </c>
+      <c r="K37" t="n">
         <v>3</v>
       </c>
-      <c r="J37" t="n">
-        <v>4</v>
-      </c>
-      <c r="K37" t="n">
-        <v>1</v>
-      </c>
-      <c r="L37" t="b">
-        <v>0</v>
-      </c>
-      <c r="M37" t="b">
-        <v>0</v>
-      </c>
-      <c r="N37" t="b">
-        <v>0</v>
-      </c>
-      <c r="O37" t="b">
+      <c r="L37" t="n">
+        <v>5</v>
+      </c>
+      <c r="M37" t="n">
+        <v>1</v>
+      </c>
+      <c r="N37" t="n">
+        <v>0</v>
+      </c>
+      <c r="O37" t="n">
         <v>0</v>
       </c>
       <c r="P37" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q37" t="b">
+        <v>0</v>
+      </c>
+      <c r="R37" t="b">
+        <v>0</v>
+      </c>
+      <c r="S37" t="b">
+        <v>0</v>
+      </c>
+      <c r="T37" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2792,37 +3315,51 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G38" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H38" t="n">
+        <v>662</v>
+      </c>
+      <c r="I38" t="n">
         <v>22</v>
       </c>
-      <c r="H38" t="n">
-        <v>0</v>
-      </c>
-      <c r="I38" t="n">
+      <c r="J38" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" t="n">
         <v>4</v>
       </c>
-      <c r="J38" t="n">
-        <v>73</v>
-      </c>
-      <c r="K38" t="n">
-        <v>0</v>
-      </c>
-      <c r="L38" t="b">
-        <v>0</v>
-      </c>
-      <c r="M38" t="b">
-        <v>0</v>
-      </c>
-      <c r="N38" t="b">
-        <v>0</v>
-      </c>
-      <c r="O38" t="b">
+      <c r="L38" t="n">
+        <v>59</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" t="n">
+        <v>0</v>
+      </c>
+      <c r="O38" t="n">
         <v>0</v>
       </c>
       <c r="P38" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q38" t="b">
+        <v>0</v>
+      </c>
+      <c r="R38" t="b">
+        <v>0</v>
+      </c>
+      <c r="S38" t="b">
+        <v>0</v>
+      </c>
+      <c r="T38" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2854,37 +3391,51 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G39" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H39" t="n">
+        <v>662</v>
+      </c>
+      <c r="I39" t="n">
         <v>22</v>
       </c>
-      <c r="H39" t="n">
+      <c r="J39" t="n">
         <v>2</v>
       </c>
-      <c r="I39" t="n">
-        <v>3</v>
-      </c>
-      <c r="J39" t="n">
-        <v>9</v>
-      </c>
       <c r="K39" t="n">
-        <v>0</v>
-      </c>
-      <c r="L39" t="b">
-        <v>0</v>
-      </c>
-      <c r="M39" t="b">
-        <v>0</v>
-      </c>
-      <c r="N39" t="b">
-        <v>0</v>
-      </c>
-      <c r="O39" t="b">
+        <v>2</v>
+      </c>
+      <c r="L39" t="n">
+        <v>1</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0</v>
+      </c>
+      <c r="N39" t="n">
+        <v>0</v>
+      </c>
+      <c r="O39" t="n">
         <v>0</v>
       </c>
       <c r="P39" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q39" t="b">
+        <v>0</v>
+      </c>
+      <c r="R39" t="b">
+        <v>0</v>
+      </c>
+      <c r="S39" t="b">
+        <v>0</v>
+      </c>
+      <c r="T39" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2916,37 +3467,51 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G40" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H40" t="n">
+        <v>662</v>
+      </c>
+      <c r="I40" t="n">
         <v>22</v>
       </c>
-      <c r="H40" t="n">
+      <c r="J40" t="n">
         <v>2</v>
       </c>
-      <c r="I40" t="n">
-        <v>3</v>
-      </c>
-      <c r="J40" t="n">
-        <v>46</v>
-      </c>
       <c r="K40" t="n">
-        <v>0</v>
-      </c>
-      <c r="L40" t="b">
-        <v>0</v>
-      </c>
-      <c r="M40" t="b">
-        <v>0</v>
-      </c>
-      <c r="N40" t="b">
-        <v>0</v>
-      </c>
-      <c r="O40" t="b">
+        <v>2</v>
+      </c>
+      <c r="L40" t="n">
+        <v>1</v>
+      </c>
+      <c r="M40" t="n">
+        <v>0</v>
+      </c>
+      <c r="N40" t="n">
+        <v>0</v>
+      </c>
+      <c r="O40" t="n">
         <v>0</v>
       </c>
       <c r="P40" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q40" t="b">
+        <v>0</v>
+      </c>
+      <c r="R40" t="b">
+        <v>0</v>
+      </c>
+      <c r="S40" t="b">
+        <v>0</v>
+      </c>
+      <c r="T40" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2978,37 +3543,51 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G41" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H41" t="n">
+        <v>662</v>
+      </c>
+      <c r="I41" t="n">
         <v>7</v>
       </c>
-      <c r="H41" t="n">
-        <v>0</v>
-      </c>
-      <c r="I41" t="n">
-        <v>1</v>
-      </c>
       <c r="J41" t="n">
         <v>0</v>
       </c>
       <c r="K41" t="n">
-        <v>3159</v>
-      </c>
-      <c r="L41" t="b">
-        <v>0</v>
-      </c>
-      <c r="M41" t="b">
-        <v>0</v>
-      </c>
-      <c r="N41" t="b">
-        <v>0</v>
-      </c>
-      <c r="O41" t="b">
+        <v>1</v>
+      </c>
+      <c r="L41" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" t="n">
+        <v>662</v>
+      </c>
+      <c r="N41" t="n">
+        <v>0</v>
+      </c>
+      <c r="O41" t="n">
         <v>0</v>
       </c>
       <c r="P41" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q41" t="b">
+        <v>0</v>
+      </c>
+      <c r="R41" t="b">
+        <v>0</v>
+      </c>
+      <c r="S41" t="b">
+        <v>0</v>
+      </c>
+      <c r="T41" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3035,42 +3614,56 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>OBSERVAÇÃO</t>
+          <t>OBSERVA��O</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (, )</t>
-        </is>
-      </c>
-      <c r="G42" t="n">
+          <t xml:space="preserve"> (: )</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H42" t="n">
+        <v>662</v>
+      </c>
+      <c r="I42" t="n">
         <v>500</v>
       </c>
-      <c r="H42" t="n">
-        <v>0</v>
-      </c>
-      <c r="I42" t="n">
-        <v>2</v>
-      </c>
       <c r="J42" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="K42" t="n">
-        <v>3146</v>
-      </c>
-      <c r="L42" t="b">
-        <v>0</v>
-      </c>
-      <c r="M42" t="b">
-        <v>0</v>
-      </c>
-      <c r="N42" t="b">
-        <v>0</v>
-      </c>
-      <c r="O42" t="b">
+        <v>3</v>
+      </c>
+      <c r="L42" t="n">
+        <v>8</v>
+      </c>
+      <c r="M42" t="n">
+        <v>654</v>
+      </c>
+      <c r="N42" t="n">
+        <v>0</v>
+      </c>
+      <c r="O42" t="n">
         <v>0</v>
       </c>
       <c r="P42" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q42" t="b">
+        <v>0</v>
+      </c>
+      <c r="R42" t="b">
+        <v>0</v>
+      </c>
+      <c r="S42" t="b">
+        <v>0</v>
+      </c>
+      <c r="T42" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3097,42 +3690,56 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>chave estrangeira - gráfica onde o pedido foi originado</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>FK_GRA_PED_GRA (FOREIGN KEY, ENABLED); SYS_C001522235 (CHECK, ENABLED)</t>
-        </is>
-      </c>
-      <c r="G43" t="n">
+          <t>FK_GRA_PED_GRA (FOREIGN KEY: ENABLED)</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H43" t="n">
+        <v>662</v>
+      </c>
+      <c r="I43" t="n">
         <v>22</v>
       </c>
-      <c r="H43" t="n">
-        <v>0</v>
-      </c>
-      <c r="I43" t="n">
+      <c r="J43" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" t="n">
         <v>3</v>
       </c>
-      <c r="J43" t="n">
-        <v>1</v>
-      </c>
-      <c r="K43" t="n">
-        <v>0</v>
-      </c>
-      <c r="L43" t="b">
-        <v>0</v>
-      </c>
-      <c r="M43" t="b">
-        <v>0</v>
-      </c>
-      <c r="N43" t="b">
-        <v>0</v>
-      </c>
-      <c r="O43" t="b">
-        <v>1</v>
+      <c r="L43" t="n">
+        <v>1</v>
+      </c>
+      <c r="M43" t="n">
+        <v>0</v>
+      </c>
+      <c r="N43" t="n">
+        <v>0</v>
+      </c>
+      <c r="O43" t="n">
+        <v>0</v>
       </c>
       <c r="P43" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q43" t="b">
+        <v>0</v>
+      </c>
+      <c r="R43" t="b">
+        <v>0</v>
+      </c>
+      <c r="S43" t="b">
+        <v>1</v>
+      </c>
+      <c r="T43" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3164,37 +3771,51 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>PK_SELO (PRIMARY KEY, ENABLED); SYS_C001240603 (CHECK, ENABLED)</t>
-        </is>
-      </c>
-      <c r="G44" t="n">
+          <t>PK_SELO (PRIMARY KEY: ENABLED)- SYS_C0080233 (C: ENABLED)</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H44" t="n">
+        <v>12</v>
+      </c>
+      <c r="I44" t="n">
         <v>22</v>
       </c>
-      <c r="H44" t="n">
-        <v>0</v>
-      </c>
-      <c r="I44" t="n">
-        <v>7</v>
-      </c>
       <c r="J44" t="n">
-        <v>140121017</v>
+        <v>0</v>
       </c>
       <c r="K44" t="n">
-        <v>0</v>
-      </c>
-      <c r="L44" t="b">
-        <v>0</v>
-      </c>
-      <c r="M44" t="b">
-        <v>0</v>
-      </c>
-      <c r="N44" t="b">
-        <v>1</v>
-      </c>
-      <c r="O44" t="b">
+        <v>3</v>
+      </c>
+      <c r="L44" t="n">
+        <v>12</v>
+      </c>
+      <c r="M44" t="n">
+        <v>0</v>
+      </c>
+      <c r="N44" t="n">
+        <v>0</v>
+      </c>
+      <c r="O44" t="n">
         <v>0</v>
       </c>
       <c r="P44" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q44" t="b">
+        <v>0</v>
+      </c>
+      <c r="R44" t="b">
+        <v>1</v>
+      </c>
+      <c r="S44" t="b">
+        <v>0</v>
+      </c>
+      <c r="T44" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3226,37 +3847,51 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>FK_PED_R_SEL (FOREIGN KEY, ENABLED); SYS_C001348709 (CHECK, ENABLED)</t>
-        </is>
-      </c>
-      <c r="G45" t="n">
+          <t>FK_PED_R_SEL (FOREIGN KEY: ENABLED)- SYS_C0080234 (C: ENABLED)</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H45" t="n">
+        <v>12</v>
+      </c>
+      <c r="I45" t="n">
         <v>22</v>
       </c>
-      <c r="H45" t="n">
-        <v>0</v>
-      </c>
-      <c r="I45" t="n">
-        <v>4</v>
-      </c>
       <c r="J45" t="n">
-        <v>1888</v>
+        <v>0</v>
       </c>
       <c r="K45" t="n">
-        <v>0</v>
-      </c>
-      <c r="L45" t="b">
-        <v>0</v>
-      </c>
-      <c r="M45" t="b">
-        <v>0</v>
-      </c>
-      <c r="N45" t="b">
-        <v>0</v>
-      </c>
-      <c r="O45" t="b">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="L45" t="n">
+        <v>5</v>
+      </c>
+      <c r="M45" t="n">
+        <v>0</v>
+      </c>
+      <c r="N45" t="n">
+        <v>0</v>
+      </c>
+      <c r="O45" t="n">
+        <v>0</v>
       </c>
       <c r="P45" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q45" t="b">
+        <v>0</v>
+      </c>
+      <c r="R45" t="b">
+        <v>0</v>
+      </c>
+      <c r="S45" t="b">
+        <v>1</v>
+      </c>
+      <c r="T45" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3288,37 +3923,51 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>SYS_C001348710 (CHECK, ENABLED)</t>
-        </is>
-      </c>
-      <c r="G46" t="n">
+          <t>SYS_C0080235 (C: ENABLED)</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H46" t="n">
+        <v>12</v>
+      </c>
+      <c r="I46" t="n">
         <v>20</v>
       </c>
-      <c r="H46" t="n">
-        <v>0</v>
-      </c>
-      <c r="I46" t="n">
-        <v>12</v>
-      </c>
       <c r="J46" t="n">
-        <v>112164864</v>
+        <v>0</v>
       </c>
       <c r="K46" t="n">
-        <v>0</v>
-      </c>
-      <c r="L46" t="b">
-        <v>0</v>
-      </c>
-      <c r="M46" t="b">
-        <v>0</v>
-      </c>
-      <c r="N46" t="b">
-        <v>0</v>
-      </c>
-      <c r="O46" t="b">
+        <v>3</v>
+      </c>
+      <c r="L46" t="n">
+        <v>3</v>
+      </c>
+      <c r="M46" t="n">
+        <v>0</v>
+      </c>
+      <c r="N46" t="n">
+        <v>0</v>
+      </c>
+      <c r="O46" t="n">
         <v>0</v>
       </c>
       <c r="P46" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q46" t="b">
+        <v>0</v>
+      </c>
+      <c r="R46" t="b">
+        <v>0</v>
+      </c>
+      <c r="S46" t="b">
+        <v>0</v>
+      </c>
+      <c r="T46" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3345,42 +3994,56 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Número Aleatório do SELO</t>
+          <t>N�mero Aleat�rio do SELO</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>SYS_C001348711 (CHECK, ENABLED)</t>
-        </is>
-      </c>
-      <c r="G47" t="n">
+          <t>SYS_C0080236 (C: ENABLED)</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H47" t="n">
+        <v>12</v>
+      </c>
+      <c r="I47" t="n">
         <v>8</v>
       </c>
-      <c r="H47" t="n">
-        <v>0</v>
-      </c>
-      <c r="I47" t="n">
-        <v>9</v>
-      </c>
       <c r="J47" t="n">
-        <v>107462656</v>
+        <v>0</v>
       </c>
       <c r="K47" t="n">
-        <v>0</v>
-      </c>
-      <c r="L47" t="b">
-        <v>0</v>
-      </c>
-      <c r="M47" t="b">
-        <v>0</v>
-      </c>
-      <c r="N47" t="b">
-        <v>0</v>
-      </c>
-      <c r="O47" t="b">
+        <v>2</v>
+      </c>
+      <c r="L47" t="n">
+        <v>4</v>
+      </c>
+      <c r="M47" t="n">
+        <v>0</v>
+      </c>
+      <c r="N47" t="n">
+        <v>0</v>
+      </c>
+      <c r="O47" t="n">
         <v>0</v>
       </c>
       <c r="P47" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q47" t="b">
+        <v>0</v>
+      </c>
+      <c r="R47" t="b">
+        <v>0</v>
+      </c>
+      <c r="S47" t="b">
+        <v>0</v>
+      </c>
+      <c r="T47" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3395,7 +4058,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3411,10 +4074,15 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Value</t>
         </is>
@@ -3428,10 +4096,15 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>RAW</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>Total number of tables</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3443,10 +4116,15 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>RAW</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>Total number of columns</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>46</v>
       </c>
     </row>
@@ -3458,10 +4136,15 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>RAW</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>Total number of primary key</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>4</v>
       </c>
     </row>
@@ -3473,10 +4156,15 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>RAW</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>Total number of foreign key</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3488,11 +4176,216 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>RAW</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>Total number of unique key</t>
         </is>
       </c>
-      <c r="C6" t="n">
-        <v>0</v>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>MQME017</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>RAW</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Total number of rows in schema</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>5463</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>MQME018</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>RAW</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Total number of cells in schema</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>31422</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>MQME019</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>RAW</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Total number of null values (nullable, no default) in schema</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>2305</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>MQME006</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>DERIVED</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Total number of length-required columns</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>MQME007</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>DERIVED</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Total number of NUMBER columns</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>MQME007</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>RAW</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Total rows for table GRAFICA</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>MQME007</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>RAW</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Total rows for table PEDIDO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>MQME007</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>RAW</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Total rows for table PEDIDO_FLUXO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>4459</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>MQME007</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>RAW</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Total rows for table PEDIDO_GRAFICA</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>MQME007</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>RAW</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Total rows for table SELO</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -3506,7 +4399,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3564,7 +4457,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Total number of tables with non-standard column prefixes</t>
+          <t>Columns with non-standard prefixes</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -3585,6 +4478,336 @@
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>MQME008</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>SISAGUA</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>GRAFICA</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>SEQ_GRAFICA</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>MQME008</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SISAGUA</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>GRAFICA</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>COD_CNPJ</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>MQME008</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>SISAGUA</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>GRAFICA</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>NOM_GRAFICA</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>MQME008</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>SISAGUA</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>GRAFICA</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>DAT_INICIO</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>MQME008</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>SISAGUA</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>GRAFICA</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>DAT_FIM</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>MQME008</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>SISAGUA</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>GRAFICA</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>STA_ATIVA</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>MQME008</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>SISAGUA</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>GRAFICA</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>NOM_USUARIO</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>MQME008</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>SISAGUA</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>GRAFICA</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>NOM_SENHA</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>MQME008</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>SISAGUA</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>GRAFICA</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>NOM_URL</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>MQME008</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>SISAGUA</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>PEDIDO</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>SEQ_GRAFICA</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>MQME008</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>SISAGUA</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>PEDIDO_GRAFICA</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>SEQ_GRAFICA</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3597,7 +4820,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3625,89 +4848,23 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MQME006</t>
+          <t>MQID001</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Total number of length-required columns</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>11</v>
+          <t>Table names in singular</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>100.00%</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MQME007</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Total number of NUMBER columns</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Indicator</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>MQID001</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Table names in singular</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>100.00%</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
           <t>MQID002</t>
         </is>
       </c>
@@ -3769,7 +4926,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>100.00%</t>
+          <t>76.09%</t>
         </is>
       </c>
     </row>
@@ -3832,7 +4989,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>NUMBER columns with valid scale</t>
+          <t>Columns with valid num_distinct</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -3849,29 +5006,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Columns with valid num_distinct</t>
+          <t>Columns with num_nulls</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>100.00%</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>MQID011</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Columns with valid num_nulls</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>100.00%</t>
+          <t>92.66%</t>
         </is>
       </c>
     </row>

</xml_diff>